<commit_message>
Memoli 2015 + 2016 model fits
vRNA fits, plotting out serum cytokines. Too sparse, no dynamics, shorter than viral dynamics.
</commit_message>
<xml_diff>
--- a/Data/Memoli.xlsx
+++ b/Data/Memoli.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveutk-my.sharepoint.com/personal/jweave49_uthsc_edu/Documents/GitHub/VirtualPatient/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{7E127BD8-5C17-420D-A6B9-31ACAE01DDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5086CFA-3A1D-4BD7-9D16-8F6BE1A98DF7}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{7E127BD8-5C17-420D-A6B9-31ACAE01DDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11F19734-3E9B-4DEA-BE11-499E9BBF2DB5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{5E827E76-6625-47FF-8BB1-49D1DDE9ED7B}"/>
+    <workbookView xWindow="-15645" yWindow="2115" windowWidth="12225" windowHeight="11835" xr2:uid="{5E827E76-6625-47FF-8BB1-49D1DDE9ED7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="2015" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>V</t>
   </si>
@@ -47,7 +47,28 @@
     <t>VOLUNTEER</t>
   </si>
   <si>
-    <t>Mean</t>
+    <t>GCSF</t>
+  </si>
+  <si>
+    <t>IFNG</t>
+  </si>
+  <si>
+    <t>IL6</t>
+  </si>
+  <si>
+    <t>TNFA</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>2016LoHAI</t>
+  </si>
+  <si>
+    <t>2016HiHAI</t>
+  </si>
+  <si>
+    <t>2015Mean</t>
   </si>
 </sst>
 </file>
@@ -471,15 +492,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2F975C-5CF1-4CD9-BB4F-3E47C9479E82}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -489,10 +510,25 @@
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -500,10 +536,25 @@
       <c r="C2" s="1">
         <v>160.8773852430167</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <v>2.07214710083425</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.8787231309594017</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.83520630659662332</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.3160853443758567</v>
+      </c>
+      <c r="H2">
+        <v>0.114293580562431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -511,10 +562,25 @@
       <c r="C3" s="3">
         <v>3082.6881368352124</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>2.0925756194889131</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.9180116497471442</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.97285842091697461</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.3224607408897178</v>
+      </c>
+      <c r="H3">
+        <v>0.58277995074171596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -522,10 +588,13 @@
       <c r="C4" s="3">
         <v>16880.13218681989</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1.8232716956400701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -533,10 +602,25 @@
       <c r="C5" s="1">
         <v>16906.325480665259</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <v>2.1704207543291636</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.7665154267369445</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.99234476666539417</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.5689442921407151</v>
+      </c>
+      <c r="H5">
+        <v>3.49150548993437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -544,10 +628,13 @@
       <c r="C6" s="1">
         <v>1948.7584048508834</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>3.6574364744715799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -555,10 +642,25 @@
       <c r="C7" s="1">
         <v>47481.233646657769</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>1.8875998384572792</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.6309935214254174</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.99124375149873178</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.4213580892700912</v>
+      </c>
+      <c r="H7">
+        <v>3.42700586849893</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -566,10 +668,13 @@
       <c r="C8" s="3">
         <v>2401.9275036040444</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>2.1115822801856599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -577,10 +682,13 @@
       <c r="C9" s="3">
         <v>1274.9864685107586</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1.8289696160786599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -588,15 +696,208 @@
       <c r="C10" s="1">
         <v>267.9401851121255</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0.67005030569462798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.60651430315689803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1122.948171278714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4515.192378428178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
+      <c r="C14">
+        <v>14397.045636220895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>19398.573030675019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>9053.8757952982342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>1240.2955338330044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2">
+        <v>541.7675012235203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5417.6750122352041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>43.680516977211418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>248.704391122673</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6083.7682475720385</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>139.27876015629599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>187.6641408787614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>13.927876015629595</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="2">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>